<commit_message>
Reading cards definition, initial setup, graphics changes
</commit_message>
<xml_diff>
--- a/PySplendor/resources/Cards.xlsx
+++ b/PySplendor/resources/Cards.xlsx
@@ -4,21 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="12915" windowHeight="7740"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="12915" windowHeight="7740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="4" r:id="rId2"/>
     <sheet name="3" sheetId="6" r:id="rId3"/>
+    <sheet name="cards" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
   <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>deck</t>
   </si>
 </sst>
 </file>
@@ -409,9 +413,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,19 +449,46 @@
       <c r="A2" s="1">
         <v>2</v>
       </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="5">
         <v>4</v>
       </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
       <c r="F3" s="5">
         <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -470,11 +501,17 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="5">
         <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -487,17 +524,35 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="5">
         <v>4</v>
       </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
@@ -506,20 +561,35 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="5">
         <v>4</v>
       </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
@@ -532,30 +602,69 @@
       <c r="F8" s="5">
         <v>4</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="5">
         <v>4</v>
       </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
       </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
       <c r="E11" s="1">
         <v>4</v>
       </c>
@@ -567,6 +676,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -576,33 +688,69 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
       <c r="F12" s="3">
         <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
       <c r="F13" s="3">
         <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
       <c r="F14" s="3">
         <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
@@ -614,26 +762,41 @@
       </c>
       <c r="F15" s="3">
         <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
@@ -645,6 +808,9 @@
       </c>
       <c r="F17" s="3">
         <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -660,24 +826,54 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
       <c r="F18" s="6">
         <v>5</v>
       </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
       <c r="D19" s="1">
         <v>2</v>
       </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
       <c r="F19" s="6">
         <v>5</v>
       </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
       <c r="C20" s="1">
         <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
       </c>
       <c r="F20" s="6">
         <v>5</v>
@@ -690,14 +886,23 @@
       <c r="A21" s="1">
         <v>1</v>
       </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
       <c r="F21" s="6">
         <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -707,11 +912,20 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
       <c r="E22" s="1">
         <v>1</v>
       </c>
       <c r="F22" s="6">
         <v>5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,8 +941,14 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
       <c r="F23" s="6">
         <v>5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -738,24 +958,66 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
       <c r="F24" s="6">
         <v>5</v>
       </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
       <c r="B25" s="1">
         <v>3</v>
       </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
       <c r="F25" s="6">
         <v>5</v>
       </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
       <c r="E26" s="1">
         <v>3</v>
       </c>
       <c r="F26" s="4">
         <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -765,6 +1027,9 @@
       <c r="B27" s="1">
         <v>1</v>
       </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
@@ -774,16 +1039,31 @@
       <c r="F27" s="4">
         <v>3</v>
       </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
       <c r="B28" s="1">
         <v>2</v>
       </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" s="4">
         <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,6 +1073,9 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
@@ -801,6 +1084,9 @@
       </c>
       <c r="F29" s="4">
         <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -813,11 +1099,29 @@
       <c r="C30" s="1">
         <v>1</v>
       </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
       <c r="F30" s="4">
         <v>3</v>
       </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
@@ -826,6 +1130,9 @@
       </c>
       <c r="F31" s="4">
         <v>3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -835,17 +1142,38 @@
       <c r="B32" s="1">
         <v>2</v>
       </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
       <c r="F32" s="4">
         <v>3</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
       <c r="F33" s="4">
         <v>3</v>
       </c>
@@ -857,14 +1185,29 @@
       <c r="A34" s="1">
         <v>2</v>
       </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
       <c r="D34" s="1">
         <v>2</v>
       </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
       <c r="F34" s="2">
         <v>1</v>
       </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
@@ -880,19 +1223,43 @@
       <c r="F35" s="2">
         <v>1</v>
       </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
       <c r="F36" s="2">
         <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1</v>
       </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
@@ -902,19 +1269,37 @@
       <c r="F37" s="2">
         <v>1</v>
       </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
       <c r="F38" s="2">
         <v>1</v>
       </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
@@ -930,11 +1315,26 @@
       <c r="F39" s="2">
         <v>1</v>
       </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
       <c r="D40" s="1">
         <v>4</v>
       </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
       <c r="F40" s="2">
         <v>1</v>
       </c>
@@ -943,9 +1343,15 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
       <c r="B41" s="1">
         <v>1</v>
       </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
       <c r="D41" s="1">
         <v>2</v>
       </c>
@@ -954,6 +1360,9 @@
       </c>
       <c r="F41" s="2">
         <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +1376,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,9 +1407,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" s="1">
         <v>6</v>
       </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
       <c r="F2" s="5">
         <v>4</v>
       </c>
@@ -1012,6 +1433,15 @@
       <c r="A3" s="1">
         <v>5</v>
       </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
       <c r="E3" s="1">
         <v>3</v>
       </c>
@@ -1029,6 +1459,12 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
@@ -1043,11 +1479,17 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
       </c>
       <c r="F5" s="5">
         <v>4</v>
@@ -1060,6 +1502,18 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
@@ -1074,6 +1528,12 @@
       <c r="B7" s="1">
         <v>3</v>
       </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
@@ -1085,6 +1545,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -1102,9 +1568,21 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
       <c r="B9" s="1">
         <v>5</v>
       </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
       <c r="F9" s="3">
         <v>2</v>
       </c>
@@ -1113,12 +1591,21 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
       </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
@@ -1127,6 +1614,12 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
@@ -1144,9 +1637,21 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
       <c r="B12" s="1">
         <v>6</v>
       </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
@@ -1161,9 +1666,15 @@
       <c r="B13" s="1">
         <v>2</v>
       </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
       <c r="F13" s="3">
         <v>2</v>
       </c>
@@ -1172,9 +1683,21 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
       <c r="D14" s="1">
         <v>5</v>
       </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
       <c r="F14" s="6">
         <v>5</v>
       </c>
@@ -1183,6 +1706,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -1192,6 +1718,9 @@
       <c r="D15" s="1">
         <v>3</v>
       </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
       <c r="F15" s="6">
         <v>5</v>
       </c>
@@ -1200,8 +1729,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
       <c r="B16" s="1">
         <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -1226,6 +1761,12 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
       <c r="F17" s="6">
         <v>5</v>
       </c>
@@ -1240,6 +1781,15 @@
       <c r="B18" s="1">
         <v>5</v>
       </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
       <c r="F18" s="6">
         <v>5</v>
       </c>
@@ -1248,6 +1798,18 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
       <c r="E19" s="1">
         <v>6</v>
       </c>
@@ -1259,9 +1821,21 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
       <c r="C20" s="1">
         <v>6</v>
       </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
       <c r="F20" s="4">
         <v>3</v>
       </c>
@@ -1270,11 +1844,20 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
       <c r="C21" s="1">
         <v>3</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
       </c>
       <c r="F21" s="4">
         <v>3</v>
@@ -1287,6 +1870,12 @@
       <c r="A22" s="1">
         <v>1</v>
       </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
@@ -1301,8 +1890,20 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
       <c r="C23" s="1">
         <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <v>3</v>
@@ -1321,6 +1922,12 @@
       <c r="C24" s="1">
         <v>2</v>
       </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
       <c r="F24" s="4">
         <v>3</v>
       </c>
@@ -1329,11 +1936,17 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
       <c r="B25" s="1">
         <v>3</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -1349,6 +1962,18 @@
       <c r="A26" s="1">
         <v>6</v>
       </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
@@ -1360,9 +1985,15 @@
       <c r="A27" s="1">
         <v>2</v>
       </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
       <c r="C27" s="1">
         <v>3</v>
       </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
       <c r="E27" s="1">
         <v>3</v>
       </c>
@@ -1374,6 +2005,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
       <c r="D28" s="1">
         <v>3</v>
       </c>
@@ -1388,6 +2028,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
@@ -1397,6 +2040,9 @@
       <c r="D29" s="1">
         <v>1</v>
       </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
       <c r="F29" s="2">
         <v>1</v>
       </c>
@@ -1405,6 +2051,18 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
       <c r="E30" s="1">
         <v>5</v>
       </c>
@@ -1418,6 +2076,12 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
@@ -1443,7 +2107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,6 +2147,9 @@
       <c r="C2" s="1">
         <v>3</v>
       </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
       <c r="E2" s="1">
         <v>3</v>
       </c>
@@ -1494,6 +2161,18 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
@@ -1505,6 +2184,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
@@ -1522,6 +2210,12 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
@@ -1539,6 +2233,9 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
@@ -1556,6 +2253,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1565,6 +2265,9 @@
       <c r="D7" s="1">
         <v>3</v>
       </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
       <c r="F7" s="3">
         <v>2</v>
       </c>
@@ -1573,9 +2276,21 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
       <c r="C8" s="1">
         <v>7</v>
       </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
       <c r="F8" s="3">
         <v>2</v>
       </c>
@@ -1584,11 +2299,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <v>2</v>
@@ -1601,6 +2325,18 @@
       <c r="A10" s="1">
         <v>7</v>
       </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
       <c r="F10" s="6">
         <v>5</v>
       </c>
@@ -1615,6 +2351,12 @@
       <c r="B11" s="1">
         <v>3</v>
       </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
@@ -1637,6 +2379,9 @@
       </c>
       <c r="D12" s="1">
         <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
       </c>
       <c r="F12" s="6">
         <v>5</v>
@@ -1649,6 +2394,15 @@
       <c r="A13" s="1">
         <v>7</v>
       </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
       <c r="E13" s="1">
         <v>3</v>
       </c>
@@ -1666,6 +2420,9 @@
       <c r="B14" s="1">
         <v>3</v>
       </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
@@ -1680,12 +2437,21 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
       <c r="C15" s="1">
         <v>3</v>
       </c>
       <c r="D15" s="1">
         <v>7</v>
       </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
       <c r="F15" s="4">
         <v>3</v>
       </c>
@@ -1694,6 +2460,12 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
@@ -1711,9 +2483,21 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
       <c r="D17" s="1">
         <v>7</v>
       </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
       <c r="F17" s="4">
         <v>3</v>
       </c>
@@ -1731,6 +2515,12 @@
       <c r="C18" s="1">
         <v>3</v>
       </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
@@ -1739,9 +2529,21 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
       <c r="B19" s="1">
         <v>7</v>
       </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
@@ -1750,6 +2552,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -1776,11 +2581,2400 @@
       <c r="B21" s="1">
         <v>7</v>
       </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" s="1">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <v>5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="4">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="5">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2</v>
+      </c>
+      <c r="F44" s="5">
+        <v>4</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <v>4</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>4</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>2</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+      <c r="F47" s="5">
+        <v>4</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2</v>
+      </c>
+      <c r="H48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2</v>
+      </c>
+      <c r="H49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>2</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3</v>
+      </c>
+      <c r="H52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>2</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>5</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="6">
+        <v>5</v>
+      </c>
+      <c r="G54" s="1">
+        <v>2</v>
+      </c>
+      <c r="H54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6">
+        <v>5</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
+      <c r="F56" s="6">
+        <v>5</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>2</v>
+      </c>
+      <c r="B57" s="1">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="6">
+        <v>5</v>
+      </c>
+      <c r="G57" s="1">
+        <v>2</v>
+      </c>
+      <c r="H57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>3</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="6">
+        <v>5</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>6</v>
+      </c>
+      <c r="F59" s="6">
+        <v>5</v>
+      </c>
+      <c r="G59" s="1">
+        <v>3</v>
+      </c>
+      <c r="H59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <v>3</v>
+      </c>
+      <c r="G60" s="1">
+        <v>3</v>
+      </c>
+      <c r="H60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>3</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
+        <v>3</v>
+      </c>
+      <c r="G61" s="1">
+        <v>2</v>
+      </c>
+      <c r="H61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>4</v>
+      </c>
+      <c r="F62" s="4">
+        <v>3</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2</v>
+      </c>
+      <c r="H62" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>5</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="4">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1">
+        <v>2</v>
+      </c>
+      <c r="H63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>3</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="4">
+        <v>3</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>3</v>
+      </c>
+      <c r="F65" s="4">
+        <v>3</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>6</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>3</v>
+      </c>
+      <c r="H66" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>2</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>3</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>3</v>
+      </c>
+      <c r="E68" s="1">
+        <v>5</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>2</v>
+      </c>
+      <c r="H68" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2</v>
+      </c>
+      <c r="C69" s="1">
+        <v>4</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>2</v>
+      </c>
+      <c r="H69" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>5</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>2</v>
+      </c>
+      <c r="H70" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2</v>
+      </c>
+      <c r="E71" s="1">
+        <v>3</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>5</v>
+      </c>
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1">
+        <v>3</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>3</v>
+      </c>
+      <c r="F72" s="5">
+        <v>4</v>
+      </c>
+      <c r="G72" s="1">
+        <v>3</v>
+      </c>
+      <c r="H72" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>7</v>
+      </c>
+      <c r="F73" s="5">
+        <v>4</v>
+      </c>
+      <c r="G73" s="1">
+        <v>4</v>
+      </c>
+      <c r="H73" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1">
+        <v>3</v>
+      </c>
+      <c r="E74" s="1">
+        <v>7</v>
+      </c>
+      <c r="F74" s="5">
+        <v>4</v>
+      </c>
+      <c r="G74" s="1">
+        <v>5</v>
+      </c>
+      <c r="H74" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>3</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1">
+        <v>6</v>
+      </c>
+      <c r="F75" s="5">
+        <v>4</v>
+      </c>
+      <c r="G75" s="1">
+        <v>4</v>
+      </c>
+      <c r="H75" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>3</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1">
+        <v>5</v>
+      </c>
+      <c r="E76" s="1">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3">
+        <v>2</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3</v>
+      </c>
+      <c r="H76" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0</v>
+      </c>
+      <c r="F77" s="3">
+        <v>2</v>
+      </c>
+      <c r="G77" s="1">
+        <v>4</v>
+      </c>
+      <c r="H77" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>7</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>2</v>
+      </c>
+      <c r="G78" s="1">
+        <v>4</v>
+      </c>
+      <c r="H78" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1">
+        <v>3</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0</v>
+      </c>
+      <c r="F79" s="3">
+        <v>2</v>
+      </c>
+      <c r="G79" s="1">
+        <v>5</v>
+      </c>
+      <c r="H79" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>7</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="6">
+        <v>5</v>
+      </c>
+      <c r="G80" s="1">
+        <v>4</v>
+      </c>
+      <c r="H80" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>6</v>
+      </c>
+      <c r="B81" s="1">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>3</v>
+      </c>
+      <c r="F81" s="6">
+        <v>5</v>
+      </c>
+      <c r="G81" s="1">
+        <v>4</v>
+      </c>
+      <c r="H81" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>3</v>
+      </c>
+      <c r="B82" s="1">
+        <v>5</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="6">
+        <v>5</v>
+      </c>
+      <c r="G82" s="1">
+        <v>3</v>
+      </c>
+      <c r="H82" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>7</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>3</v>
+      </c>
+      <c r="F83" s="6">
+        <v>5</v>
+      </c>
+      <c r="G83" s="1">
+        <v>5</v>
+      </c>
+      <c r="H83" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>3</v>
+      </c>
+      <c r="B84" s="1">
+        <v>3</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>3</v>
+      </c>
+      <c r="E84" s="1">
+        <v>5</v>
+      </c>
+      <c r="F84" s="4">
+        <v>3</v>
+      </c>
+      <c r="G84" s="1">
+        <v>3</v>
+      </c>
+      <c r="H84" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1">
+        <v>7</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0</v>
+      </c>
+      <c r="F85" s="4">
+        <v>3</v>
+      </c>
+      <c r="G85" s="1">
+        <v>5</v>
+      </c>
+      <c r="H85" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1">
+        <v>3</v>
+      </c>
+      <c r="D86" s="1">
+        <v>6</v>
+      </c>
+      <c r="E86" s="1">
+        <v>3</v>
+      </c>
+      <c r="F86" s="4">
+        <v>3</v>
+      </c>
+      <c r="G86" s="1">
+        <v>4</v>
+      </c>
+      <c r="H86" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1">
+        <v>7</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0</v>
+      </c>
+      <c r="F87" s="4">
+        <v>3</v>
+      </c>
+      <c r="G87" s="1">
+        <v>4</v>
+      </c>
+      <c r="H87" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>3</v>
+      </c>
+      <c r="B88" s="1">
+        <v>6</v>
+      </c>
+      <c r="C88" s="1">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1">
+        <v>4</v>
+      </c>
+      <c r="H88" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1">
+        <v>7</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1">
+        <v>4</v>
+      </c>
+      <c r="H89" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1">
+        <v>3</v>
+      </c>
+      <c r="C90" s="1">
+        <v>5</v>
+      </c>
+      <c r="D90" s="1">
+        <v>3</v>
+      </c>
+      <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3</v>
+      </c>
+      <c r="H90" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>3</v>
+      </c>
+      <c r="B91" s="1">
+        <v>7</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1">
+        <v>5</v>
+      </c>
+      <c r="H91" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>